<commit_message>
Able to find the operator at correct location
</commit_message>
<xml_diff>
--- a/Resources/map/mapJSON/0-1.xlsx
+++ b/Resources/map/mapJSON/0-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\program\OOPL\ArkNights\Resources\map\mapJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01D8FB2-22F3-471B-81DA-F79CACB3E09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C783185-4B51-4187-9627-9A2A40E953BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E80FDADB-74A6-47AD-8510-938BF40B829B}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -571,7 +571,7 @@
         <v>232</v>
       </c>
       <c r="C2">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>334</v>
       </c>
       <c r="C3">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>436</v>
       </c>
       <c r="C4">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>538</v>
       </c>
       <c r="C5">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
         <v>640</v>
       </c>
       <c r="C6">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>742</v>
       </c>
       <c r="C7">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
         <v>844</v>
       </c>
       <c r="C8">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>946</v>
       </c>
       <c r="C9">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
         <v>1048</v>
       </c>
       <c r="C10">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>